<commit_message>
Lots of minor edits, nearly ready...
</commit_message>
<xml_diff>
--- a/tables/Table1.xlsx
+++ b/tables/Table1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Strong Gun</t>
-  </si>
-  <si>
-    <t>Weak Gun</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Firing Spread (degrees)</t>
   </si>
@@ -34,12 +28,6 @@
     <t>Muzzle flash</t>
   </si>
   <si>
-    <t>Time to fire (frames)</t>
-  </si>
-  <si>
-    <t>[NOTE: HARD TO TELL FROM SLADE3. EASIER JUST TO TIME IT MYSELF.]</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -56,6 +44,15 @@
   </si>
   <si>
     <t>Modest</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>Rate of Fire (rounds per minute)</t>
   </si>
 </sst>
 </file>
@@ -153,7 +150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,7 +185,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,37 +394,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>155</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -436,9 +436,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0.25</v>
@@ -447,48 +447,48 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>